<commit_message>
Fixed C# native version, implemented MersenneTwister
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -274,19 +274,19 @@
                   <c:v>Java to JavaScript (GWT) on Chrome</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>TypeScript to Javascript on Firefox</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>C# to javascript on Firefox</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Dart VM (checked mode) on Dartium</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>dart2js on Chrome</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>C# native (CLR) on Windows</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>TypeScript to Javascript on Firefox</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>C# to javascript on Firefox</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Dart VM (checked mode) on Dartium</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>dart2js on Chrome</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>Java to JavaScript (GWT) on Explorer</c:v>
@@ -331,19 +331,19 @@
                   <c:v>15.535</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17.524999999999999</c:v>
+                  <c:v>24.289000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>24.289000000000001</c:v>
+                  <c:v>26.873999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>26.873999999999999</c:v>
+                  <c:v>27.3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>27.3</c:v>
+                  <c:v>35.323</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>35.323</c:v>
+                  <c:v>35.646999999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>51.56</c:v>
@@ -376,11 +376,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="178047648"/>
-        <c:axId val="178926048"/>
+        <c:axId val="180749488"/>
+        <c:axId val="181202560"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="178047648"/>
+        <c:axId val="180749488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -423,7 +423,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="178926048"/>
+        <c:crossAx val="181202560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -431,7 +431,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="178926048"/>
+        <c:axId val="181202560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -482,7 +482,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="178047648"/>
+        <c:crossAx val="180749488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="10"/>
@@ -1081,16 +1081,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>15875</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>65087</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>182562</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>92075</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>39687</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1378,7 +1378,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1415,11 +1415,11 @@
         <v>11</v>
       </c>
       <c r="C2" t="str">
-        <f t="shared" ref="C2:C17" si="0">A2&amp; " on "&amp;B2</f>
+        <f>A2&amp; " on "&amp;B2</f>
         <v>Java native JVM on Windows</v>
       </c>
       <c r="D2" s="3">
-        <f t="shared" ref="D2:D17" si="1">E2/1000</f>
+        <f>E2/1000</f>
         <v>5.4829999999999997</v>
       </c>
       <c r="E2">
@@ -1434,11 +1434,11 @@
         <v>6</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" si="0"/>
+        <f>A3&amp; " on "&amp;B3</f>
         <v>TypeScript to Javascript on Chrome</v>
       </c>
       <c r="D3" s="3">
-        <f t="shared" si="1"/>
+        <f>E3/1000</f>
         <v>8.3179999999999996</v>
       </c>
       <c r="E3">
@@ -1453,11 +1453,11 @@
         <v>0</v>
       </c>
       <c r="C4" t="str">
-        <f t="shared" si="0"/>
+        <f>A4&amp; " on "&amp;B4</f>
         <v>Dart VM (unchecked mode) on Dartium</v>
       </c>
       <c r="D4" s="3">
-        <f t="shared" si="1"/>
+        <f>E4/1000</f>
         <v>10.111000000000001</v>
       </c>
       <c r="E4">
@@ -1472,11 +1472,11 @@
         <v>6</v>
       </c>
       <c r="C5" t="str">
-        <f t="shared" si="0"/>
+        <f>A5&amp; " on "&amp;B5</f>
         <v>C# to javascript on Chrome</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" si="1"/>
+        <f>E5/1000</f>
         <v>15.045999999999999</v>
       </c>
       <c r="E5">
@@ -1491,11 +1491,11 @@
         <v>6</v>
       </c>
       <c r="C6" t="str">
-        <f t="shared" si="0"/>
+        <f>A6&amp; " on "&amp;B6</f>
         <v>Java to JavaScript (GWT) on Chrome</v>
       </c>
       <c r="D6" s="3">
-        <f t="shared" si="1"/>
+        <f>E6/1000</f>
         <v>15.535</v>
       </c>
       <c r="E6">
@@ -1504,97 +1504,97 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C7" t="str">
-        <f t="shared" si="0"/>
-        <v>C# native (CLR) on Windows</v>
+        <f>A7&amp; " on "&amp;B7</f>
+        <v>TypeScript to Javascript on Firefox</v>
       </c>
       <c r="D7" s="3">
-        <f t="shared" si="1"/>
-        <v>17.524999999999999</v>
+        <f>E7/1000</f>
+        <v>24.289000000000001</v>
       </c>
       <c r="E7">
-        <v>17525</v>
+        <v>24289</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="C8" t="str">
-        <f t="shared" si="0"/>
-        <v>TypeScript to Javascript on Firefox</v>
+        <f>A8&amp; " on "&amp;B8</f>
+        <v>C# to javascript on Firefox</v>
       </c>
       <c r="D8" s="3">
-        <f t="shared" si="1"/>
-        <v>24.289000000000001</v>
+        <f>E8/1000</f>
+        <v>26.873999999999999</v>
       </c>
       <c r="E8">
-        <v>24289</v>
+        <v>26874</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C9" t="str">
-        <f t="shared" si="0"/>
-        <v>C# to javascript on Firefox</v>
+        <f>A9&amp; " on "&amp;B9</f>
+        <v>Dart VM (checked mode) on Dartium</v>
       </c>
       <c r="D9" s="3">
-        <f t="shared" si="1"/>
-        <v>26.873999999999999</v>
+        <f>E9/1000</f>
+        <v>27.3</v>
       </c>
       <c r="E9">
-        <v>26874</v>
+        <v>27300</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C10" t="str">
-        <f t="shared" si="0"/>
-        <v>Dart VM (checked mode) on Dartium</v>
+        <f>A10&amp; " on "&amp;B10</f>
+        <v>dart2js on Chrome</v>
       </c>
       <c r="D10" s="3">
-        <f t="shared" si="1"/>
-        <v>27.3</v>
+        <f>E10/1000</f>
+        <v>35.323</v>
       </c>
       <c r="E10">
-        <v>27300</v>
+        <v>35323</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C11" t="str">
-        <f t="shared" si="0"/>
-        <v>dart2js on Chrome</v>
+        <f>A11&amp; " on "&amp;B11</f>
+        <v>C# native (CLR) on Windows</v>
       </c>
       <c r="D11" s="3">
-        <f t="shared" si="1"/>
-        <v>35.323</v>
+        <f>E11/1000</f>
+        <v>35.646999999999998</v>
       </c>
       <c r="E11">
-        <v>35323</v>
+        <v>35647</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1605,11 +1605,11 @@
         <v>1</v>
       </c>
       <c r="C12" t="str">
-        <f t="shared" si="0"/>
+        <f>A12&amp; " on "&amp;B12</f>
         <v>Java to JavaScript (GWT) on Explorer</v>
       </c>
       <c r="D12" s="3">
-        <f t="shared" si="1"/>
+        <f>E12/1000</f>
         <v>51.56</v>
       </c>
       <c r="E12">
@@ -1624,11 +1624,11 @@
         <v>1</v>
       </c>
       <c r="C13" t="str">
-        <f t="shared" si="0"/>
+        <f>A13&amp; " on "&amp;B13</f>
         <v>TypeScript to Javascript on Explorer</v>
       </c>
       <c r="D13" s="3">
-        <f t="shared" si="1"/>
+        <f>E13/1000</f>
         <v>57.438000000000002</v>
       </c>
       <c r="E13">
@@ -1643,11 +1643,11 @@
         <v>1</v>
       </c>
       <c r="C14" t="str">
-        <f t="shared" si="0"/>
+        <f>A14&amp; " on "&amp;B14</f>
         <v>C# to javascript on Explorer</v>
       </c>
       <c r="D14" s="3">
-        <f t="shared" si="1"/>
+        <f>E14/1000</f>
         <v>60.642000000000003</v>
       </c>
       <c r="E14">
@@ -1662,11 +1662,11 @@
         <v>5</v>
       </c>
       <c r="C15" t="str">
-        <f t="shared" si="0"/>
+        <f>A15&amp; " on "&amp;B15</f>
         <v>Java to JavaScript (GWT) on Firefox</v>
       </c>
       <c r="D15" s="3">
-        <f t="shared" si="1"/>
+        <f>E15/1000</f>
         <v>109.917</v>
       </c>
       <c r="E15">
@@ -1681,11 +1681,11 @@
         <v>1</v>
       </c>
       <c r="C16" t="str">
-        <f t="shared" si="0"/>
+        <f>A16&amp; " on "&amp;B16</f>
         <v>dart2js on Explorer</v>
       </c>
       <c r="D16" s="3">
-        <f t="shared" si="1"/>
+        <f>E16/1000</f>
         <v>212.096</v>
       </c>
       <c r="E16">
@@ -1700,11 +1700,11 @@
         <v>5</v>
       </c>
       <c r="C17" t="str">
-        <f t="shared" si="0"/>
+        <f>A17&amp; " on "&amp;B17</f>
         <v>dart2js on Firefox</v>
       </c>
       <c r="D17" s="3">
-        <f t="shared" si="1"/>
+        <f>E17/1000</f>
         <v>218.93</v>
       </c>
       <c r="E17">

</xml_diff>

<commit_message>
Fixed Java server Mersenne Twister, added checksum to Java
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -316,7 +316,7 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>5.4829999999999997</c:v>
+                  <c:v>5.1980000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>8.3179999999999996</c:v>
@@ -343,7 +343,7 @@
                   <c:v>35.323</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>35.646999999999998</c:v>
+                  <c:v>40.063000000000002</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>51.56</c:v>
@@ -376,11 +376,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="180749488"/>
-        <c:axId val="181202560"/>
+        <c:axId val="121390800"/>
+        <c:axId val="121391360"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="180749488"/>
+        <c:axId val="121390800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -423,7 +423,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="181202560"/>
+        <c:crossAx val="121391360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -431,7 +431,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="181202560"/>
+        <c:axId val="121391360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -482,7 +482,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="180749488"/>
+        <c:crossAx val="121390800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="10"/>
@@ -1378,7 +1378,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1415,15 +1415,15 @@
         <v>11</v>
       </c>
       <c r="C2" t="str">
-        <f>A2&amp; " on "&amp;B2</f>
+        <f t="shared" ref="C2:C17" si="0">A2&amp; " on "&amp;B2</f>
         <v>Java native JVM on Windows</v>
       </c>
       <c r="D2" s="3">
-        <f>E2/1000</f>
-        <v>5.4829999999999997</v>
+        <f t="shared" ref="D2:D17" si="1">E2/1000</f>
+        <v>5.1980000000000004</v>
       </c>
       <c r="E2">
-        <v>5483</v>
+        <v>5198</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1434,11 +1434,11 @@
         <v>6</v>
       </c>
       <c r="C3" t="str">
-        <f>A3&amp; " on "&amp;B3</f>
+        <f t="shared" si="0"/>
         <v>TypeScript to Javascript on Chrome</v>
       </c>
       <c r="D3" s="3">
-        <f>E3/1000</f>
+        <f t="shared" si="1"/>
         <v>8.3179999999999996</v>
       </c>
       <c r="E3">
@@ -1453,11 +1453,11 @@
         <v>0</v>
       </c>
       <c r="C4" t="str">
-        <f>A4&amp; " on "&amp;B4</f>
+        <f t="shared" si="0"/>
         <v>Dart VM (unchecked mode) on Dartium</v>
       </c>
       <c r="D4" s="3">
-        <f>E4/1000</f>
+        <f t="shared" si="1"/>
         <v>10.111000000000001</v>
       </c>
       <c r="E4">
@@ -1472,11 +1472,11 @@
         <v>6</v>
       </c>
       <c r="C5" t="str">
-        <f>A5&amp; " on "&amp;B5</f>
+        <f t="shared" si="0"/>
         <v>C# to javascript on Chrome</v>
       </c>
       <c r="D5" s="3">
-        <f>E5/1000</f>
+        <f t="shared" si="1"/>
         <v>15.045999999999999</v>
       </c>
       <c r="E5">
@@ -1491,11 +1491,11 @@
         <v>6</v>
       </c>
       <c r="C6" t="str">
-        <f>A6&amp; " on "&amp;B6</f>
+        <f t="shared" si="0"/>
         <v>Java to JavaScript (GWT) on Chrome</v>
       </c>
       <c r="D6" s="3">
-        <f>E6/1000</f>
+        <f t="shared" si="1"/>
         <v>15.535</v>
       </c>
       <c r="E6">
@@ -1510,11 +1510,11 @@
         <v>5</v>
       </c>
       <c r="C7" t="str">
-        <f>A7&amp; " on "&amp;B7</f>
+        <f t="shared" si="0"/>
         <v>TypeScript to Javascript on Firefox</v>
       </c>
       <c r="D7" s="3">
-        <f>E7/1000</f>
+        <f t="shared" si="1"/>
         <v>24.289000000000001</v>
       </c>
       <c r="E7">
@@ -1529,11 +1529,11 @@
         <v>5</v>
       </c>
       <c r="C8" t="str">
-        <f>A8&amp; " on "&amp;B8</f>
+        <f t="shared" si="0"/>
         <v>C# to javascript on Firefox</v>
       </c>
       <c r="D8" s="3">
-        <f>E8/1000</f>
+        <f t="shared" si="1"/>
         <v>26.873999999999999</v>
       </c>
       <c r="E8">
@@ -1548,11 +1548,11 @@
         <v>0</v>
       </c>
       <c r="C9" t="str">
-        <f>A9&amp; " on "&amp;B9</f>
+        <f t="shared" si="0"/>
         <v>Dart VM (checked mode) on Dartium</v>
       </c>
       <c r="D9" s="3">
-        <f>E9/1000</f>
+        <f t="shared" si="1"/>
         <v>27.3</v>
       </c>
       <c r="E9">
@@ -1567,11 +1567,11 @@
         <v>6</v>
       </c>
       <c r="C10" t="str">
-        <f>A10&amp; " on "&amp;B10</f>
+        <f t="shared" si="0"/>
         <v>dart2js on Chrome</v>
       </c>
       <c r="D10" s="3">
-        <f>E10/1000</f>
+        <f t="shared" si="1"/>
         <v>35.323</v>
       </c>
       <c r="E10">
@@ -1586,15 +1586,15 @@
         <v>11</v>
       </c>
       <c r="C11" t="str">
-        <f>A11&amp; " on "&amp;B11</f>
+        <f t="shared" si="0"/>
         <v>C# native (CLR) on Windows</v>
       </c>
       <c r="D11" s="3">
-        <f>E11/1000</f>
-        <v>35.646999999999998</v>
+        <f t="shared" si="1"/>
+        <v>40.063000000000002</v>
       </c>
       <c r="E11">
-        <v>35647</v>
+        <v>40063</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1605,11 +1605,11 @@
         <v>1</v>
       </c>
       <c r="C12" t="str">
-        <f>A12&amp; " on "&amp;B12</f>
+        <f t="shared" si="0"/>
         <v>Java to JavaScript (GWT) on Explorer</v>
       </c>
       <c r="D12" s="3">
-        <f>E12/1000</f>
+        <f t="shared" si="1"/>
         <v>51.56</v>
       </c>
       <c r="E12">
@@ -1624,11 +1624,11 @@
         <v>1</v>
       </c>
       <c r="C13" t="str">
-        <f>A13&amp; " on "&amp;B13</f>
+        <f t="shared" si="0"/>
         <v>TypeScript to Javascript on Explorer</v>
       </c>
       <c r="D13" s="3">
-        <f>E13/1000</f>
+        <f t="shared" si="1"/>
         <v>57.438000000000002</v>
       </c>
       <c r="E13">
@@ -1643,11 +1643,11 @@
         <v>1</v>
       </c>
       <c r="C14" t="str">
-        <f>A14&amp; " on "&amp;B14</f>
+        <f t="shared" si="0"/>
         <v>C# to javascript on Explorer</v>
       </c>
       <c r="D14" s="3">
-        <f>E14/1000</f>
+        <f t="shared" si="1"/>
         <v>60.642000000000003</v>
       </c>
       <c r="E14">
@@ -1662,11 +1662,11 @@
         <v>5</v>
       </c>
       <c r="C15" t="str">
-        <f>A15&amp; " on "&amp;B15</f>
+        <f t="shared" si="0"/>
         <v>Java to JavaScript (GWT) on Firefox</v>
       </c>
       <c r="D15" s="3">
-        <f>E15/1000</f>
+        <f t="shared" si="1"/>
         <v>109.917</v>
       </c>
       <c r="E15">
@@ -1681,11 +1681,11 @@
         <v>1</v>
       </c>
       <c r="C16" t="str">
-        <f>A16&amp; " on "&amp;B16</f>
+        <f t="shared" si="0"/>
         <v>dart2js on Explorer</v>
       </c>
       <c r="D16" s="3">
-        <f>E16/1000</f>
+        <f t="shared" si="1"/>
         <v>212.096</v>
       </c>
       <c r="E16">
@@ -1700,11 +1700,11 @@
         <v>5</v>
       </c>
       <c r="C17" t="str">
-        <f>A17&amp; " on "&amp;B17</f>
+        <f t="shared" si="0"/>
         <v>dart2js on Firefox</v>
       </c>
       <c r="D17" s="3">
-        <f>E17/1000</f>
+        <f t="shared" si="1"/>
         <v>218.93</v>
       </c>
       <c r="E17">

</xml_diff>

<commit_message>
Updated to latest Dart, C#, TypeScript
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12150"/>
   </bookViews>
   <sheets>
-    <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
+    <sheet name="12-apr-2015" sheetId="2" r:id="rId1"/>
+    <sheet name="31-aug-2014" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="17">
   <si>
     <t>Dartium</t>
   </si>
@@ -73,6 +74,9 @@
   <si>
     <t>Java native JVM</t>
   </si>
+  <si>
+    <t>12-apr-2015 (browser only update)</t>
+  </si>
 </sst>
 </file>
 
@@ -118,13 +122,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -234,7 +247,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Foglio1!$D$1</c:f>
+              <c:f>'12-apr-2015'!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -255,35 +268,35 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Foglio1!$C$2:$C$17</c:f>
+              <c:f>'12-apr-2015'!$C$3:$C$18</c:f>
               <c:strCache>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>Java native JVM on Windows</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>Dart VM (unchecked mode) on Dartium</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>TypeScript to Javascript on Firefox</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>C# to javascript on Firefox</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>TypeScript to Javascript on Chrome</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>Dart VM (unchecked mode) on Dartium</c:v>
-                </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>C# to javascript on Chrome</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>Java to JavaScript (GWT) on Chrome</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>TypeScript to Javascript on Firefox</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>C# to javascript on Firefox</c:v>
-                </c:pt>
                 <c:pt idx="7">
+                  <c:v>dart2js on Chrome</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>Dart VM (checked mode) on Dartium</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>dart2js on Chrome</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>C# native (CLR) on Windows</c:v>
@@ -301,67 +314,67 @@
                   <c:v>Java to JavaScript (GWT) on Firefox</c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>dart2js on Firefox</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>dart2js on Explorer</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>dart2js on Firefox</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$D$2:$D$17</c:f>
+              <c:f>'12-apr-2015'!$D$3:$D$18</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>5.1980000000000004</c:v>
+                  <c:v>5.5679999999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.3179999999999996</c:v>
+                  <c:v>8.3249999999999993</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.111000000000001</c:v>
+                  <c:v>12.826000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15.045999999999999</c:v>
+                  <c:v>13.523999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15.535</c:v>
+                  <c:v>13.848000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24.289000000000001</c:v>
+                  <c:v>15.005000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>26.873999999999999</c:v>
+                  <c:v>16.068999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>27.3</c:v>
+                  <c:v>17.59</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>35.323</c:v>
+                  <c:v>25.93</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>40.063000000000002</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>51.56</c:v>
+                  <c:v>54.084000000000003</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>57.438000000000002</c:v>
+                  <c:v>56.136000000000003</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>60.642000000000003</c:v>
+                  <c:v>59.939</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>109.917</c:v>
+                  <c:v>176.21899999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>212.096</c:v>
+                  <c:v>196.11600000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>218.93</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -376,11 +389,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="121390800"/>
-        <c:axId val="121391360"/>
+        <c:axId val="168527952"/>
+        <c:axId val="168529072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="121390800"/>
+        <c:axId val="168527952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -423,7 +436,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121391360"/>
+        <c:crossAx val="168529072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -431,7 +444,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="121391360"/>
+        <c:axId val="168529072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -482,7 +495,397 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121390800"/>
+        <c:crossAx val="168527952"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:minorUnit val="10"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Elapsed time (seconds)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.31898792650918634"/>
+          <c:y val="0.17171296296296296"/>
+          <c:w val="0.64494402644113935"/>
+          <c:h val="0.72088764946048411"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'31-aug-2014'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Elapsed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'31-aug-2014'!$C$2:$C$17</c:f>
+              <c:strCache>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>Java native JVM on Windows</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>TypeScript to Javascript on Chrome</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Dart VM (unchecked mode) on Dartium</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>C# to javascript on Chrome</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Java to JavaScript (GWT) on Chrome</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>TypeScript to Javascript on Firefox</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>C# to javascript on Firefox</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Dart VM (checked mode) on Dartium</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>dart2js on Chrome</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>C# native (CLR) on Windows</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Java to JavaScript (GWT) on Explorer</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>TypeScript to Javascript on Explorer</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>C# to javascript on Explorer</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Java to JavaScript (GWT) on Firefox</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>dart2js on Explorer</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>dart2js on Firefox</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'31-aug-2014'!$D$2:$D$17</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>5.1980000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.3179999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.111000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.045999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.535</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24.289000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>26.873999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>27.3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>35.323</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40.063000000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>51.56</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>57.438000000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>60.642000000000003</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>109.917</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>212.096</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>218.93</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="160965552"/>
+        <c:axId val="160966112"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="160965552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="160966112"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="160966112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="160965552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="10"/>
@@ -572,6 +975,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
@@ -1077,7 +1520,549 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>573087</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>79374</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>126999</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Grafico 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1375,10 +2360,392 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="6">
+        <v>42106</v>
+      </c>
+      <c r="E1" s="4"/>
+      <c r="F1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="5"/>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="str">
+        <f>E2</f>
+        <v>Elapsed</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="str">
+        <f>A3&amp; " on "&amp;B3</f>
+        <v>Java native JVM on Windows</v>
+      </c>
+      <c r="D3" s="3">
+        <f>E3/1000</f>
+        <v>5.5679999999999996</v>
+      </c>
+      <c r="E3">
+        <v>5568</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="str">
+        <f>A4&amp; " on "&amp;B4</f>
+        <v>Dart VM (unchecked mode) on Dartium</v>
+      </c>
+      <c r="D4" s="3">
+        <f>E4/1000</f>
+        <v>8.3249999999999993</v>
+      </c>
+      <c r="E4">
+        <v>8325</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="str">
+        <f>A5&amp; " on "&amp;B5</f>
+        <v>TypeScript to Javascript on Firefox</v>
+      </c>
+      <c r="D5" s="3">
+        <f>E5/1000</f>
+        <v>12.826000000000001</v>
+      </c>
+      <c r="E5">
+        <v>12826</v>
+      </c>
+      <c r="G5">
+        <v>12452</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="str">
+        <f>A6&amp; " on "&amp;B6</f>
+        <v>C# to javascript on Firefox</v>
+      </c>
+      <c r="D6" s="3">
+        <f>E6/1000</f>
+        <v>13.523999999999999</v>
+      </c>
+      <c r="E6">
+        <v>13524</v>
+      </c>
+      <c r="G6">
+        <v>13429</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="str">
+        <f>A7&amp; " on "&amp;B7</f>
+        <v>TypeScript to Javascript on Chrome</v>
+      </c>
+      <c r="D7" s="3">
+        <f>E7/1000</f>
+        <v>13.848000000000001</v>
+      </c>
+      <c r="E7">
+        <v>13848</v>
+      </c>
+      <c r="G7">
+        <v>8825</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="str">
+        <f>A8&amp; " on "&amp;B8</f>
+        <v>C# to javascript on Chrome</v>
+      </c>
+      <c r="D8" s="3">
+        <f>E8/1000</f>
+        <v>15.005000000000001</v>
+      </c>
+      <c r="E8">
+        <v>15005</v>
+      </c>
+      <c r="G8">
+        <v>15067</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="str">
+        <f>A9&amp; " on "&amp;B9</f>
+        <v>Java to JavaScript (GWT) on Chrome</v>
+      </c>
+      <c r="D9" s="3">
+        <f>E9/1000</f>
+        <v>16.068999999999999</v>
+      </c>
+      <c r="E9">
+        <v>16069</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="str">
+        <f>A10&amp; " on "&amp;B10</f>
+        <v>dart2js on Chrome</v>
+      </c>
+      <c r="D10" s="3">
+        <f>E10/1000</f>
+        <v>17.59</v>
+      </c>
+      <c r="E10">
+        <v>17590</v>
+      </c>
+      <c r="G10">
+        <v>25483</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" t="str">
+        <f>A11&amp; " on "&amp;B11</f>
+        <v>Dart VM (checked mode) on Dartium</v>
+      </c>
+      <c r="D11" s="3">
+        <f>E11/1000</f>
+        <v>25.93</v>
+      </c>
+      <c r="E11">
+        <v>25930</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="str">
+        <f>A12&amp; " on "&amp;B12</f>
+        <v>C# native (CLR) on Windows</v>
+      </c>
+      <c r="D12" s="3">
+        <f>E12/1000</f>
+        <v>40.063000000000002</v>
+      </c>
+      <c r="E12">
+        <v>40063</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" t="str">
+        <f>A13&amp; " on "&amp;B13</f>
+        <v>Java to JavaScript (GWT) on Explorer</v>
+      </c>
+      <c r="D13" s="3">
+        <f>E13/1000</f>
+        <v>54.084000000000003</v>
+      </c>
+      <c r="E13">
+        <v>54084</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" t="str">
+        <f>A14&amp; " on "&amp;B14</f>
+        <v>TypeScript to Javascript on Explorer</v>
+      </c>
+      <c r="D14" s="3">
+        <f>E14/1000</f>
+        <v>56.136000000000003</v>
+      </c>
+      <c r="E14">
+        <v>56136</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" t="str">
+        <f>A15&amp; " on "&amp;B15</f>
+        <v>C# to javascript on Explorer</v>
+      </c>
+      <c r="D15" s="3">
+        <f>E15/1000</f>
+        <v>59.939</v>
+      </c>
+      <c r="E15">
+        <v>59939</v>
+      </c>
+      <c r="G15">
+        <v>59939</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" t="str">
+        <f>A16&amp; " on "&amp;B16</f>
+        <v>Java to JavaScript (GWT) on Firefox</v>
+      </c>
+      <c r="D16" s="3">
+        <f>E16/1000</f>
+        <v>176.21899999999999</v>
+      </c>
+      <c r="E16">
+        <v>176219</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="str">
+        <f>A17&amp; " on "&amp;B17</f>
+        <v>dart2js on Firefox</v>
+      </c>
+      <c r="D17" s="3">
+        <f>E17/1000</f>
+        <v>196.11600000000001</v>
+      </c>
+      <c r="E17">
+        <v>196116</v>
+      </c>
+      <c r="G17">
+        <v>220610</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" t="str">
+        <f>A18&amp; " on "&amp;B18</f>
+        <v>dart2js on Explorer</v>
+      </c>
+      <c r="D18" s="3">
+        <f>E18/1000</f>
+        <v>200</v>
+      </c>
+      <c r="E18">
+        <v>200000</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A3:I18">
+    <sortCondition ref="D3:D18"/>
+  </sortState>
+  <mergeCells count="2">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed bug when running in IE
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -129,14 +129,14 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -311,13 +311,13 @@
                   <c:v>C# to javascript on Explorer</c:v>
                 </c:pt>
                 <c:pt idx="13">
+                  <c:v>dart2js on Explorer</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>Java to JavaScript (GWT) on Firefox</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>dart2js on Firefox</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>dart2js on Explorer</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -368,13 +368,13 @@
                   <c:v>59.939</c:v>
                 </c:pt>
                 <c:pt idx="13">
+                  <c:v>103.37</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>176.21899999999999</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>196.11600000000001</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -389,11 +389,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="168527952"/>
-        <c:axId val="168529072"/>
+        <c:axId val="167790224"/>
+        <c:axId val="167790784"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="168527952"/>
+        <c:axId val="167790224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -436,7 +436,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="168529072"/>
+        <c:crossAx val="167790784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -444,7 +444,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="168529072"/>
+        <c:axId val="167790784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -495,7 +495,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="168527952"/>
+        <c:crossAx val="167790224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="10"/>
@@ -779,11 +779,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="160965552"/>
-        <c:axId val="160966112"/>
+        <c:axId val="167793024"/>
+        <c:axId val="167793584"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="160965552"/>
+        <c:axId val="167793024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -826,7 +826,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="160966112"/>
+        <c:crossAx val="167793584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -834,7 +834,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="160966112"/>
+        <c:axId val="167793584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -885,7 +885,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="160965552"/>
+        <c:crossAx val="167793024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="10"/>
@@ -2362,7 +2362,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2374,14 +2376,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D1" s="6">
+      <c r="D1" s="4">
         <v>42106</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="5" t="s">
+      <c r="E1" s="5"/>
+      <c r="F1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="5"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -2668,43 +2670,40 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C16" t="str">
         <f>A16&amp; " on "&amp;B16</f>
-        <v>Java to JavaScript (GWT) on Firefox</v>
+        <v>dart2js on Explorer</v>
       </c>
       <c r="D16" s="3">
         <f>E16/1000</f>
-        <v>176.21899999999999</v>
+        <v>103.37</v>
       </c>
       <c r="E16">
-        <v>176219</v>
+        <v>103370</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B17" t="s">
         <v>5</v>
       </c>
       <c r="C17" t="str">
         <f>A17&amp; " on "&amp;B17</f>
-        <v>dart2js on Firefox</v>
+        <v>Java to JavaScript (GWT) on Firefox</v>
       </c>
       <c r="D17" s="3">
         <f>E17/1000</f>
-        <v>196.11600000000001</v>
+        <v>176.21899999999999</v>
       </c>
       <c r="E17">
-        <v>196116</v>
-      </c>
-      <c r="G17">
-        <v>220610</v>
+        <v>176219</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -2712,22 +2711,25 @@
         <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C18" t="str">
         <f>A18&amp; " on "&amp;B18</f>
-        <v>dart2js on Explorer</v>
+        <v>dart2js on Firefox</v>
       </c>
       <c r="D18" s="3">
         <f>E18/1000</f>
-        <v>200</v>
+        <v>196.11600000000001</v>
       </c>
       <c r="E18">
-        <v>200000</v>
+        <v>196116</v>
+      </c>
+      <c r="G18">
+        <v>220610</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A3:I18">
+  <sortState ref="A3:G18">
     <sortCondition ref="D3:D18"/>
   </sortState>
   <mergeCells count="2">

</xml_diff>